<commit_message>
RDM-6632: Added more test scenarios.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126ABC67-9A6A-D34B-A7B1-1630FC5CCD1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8C67D-A42D-774C-A18F-76AEBEF7844D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="282">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -904,6 +904,9 @@
   </si>
   <si>
     <t>befta.citizen.2@gmail.com</t>
+  </si>
+  <si>
+    <t>CR</t>
   </si>
 </sst>
 </file>
@@ -3354,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3473,7 +3476,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3557,7 +3560,7 @@
         <v>270</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>58</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3576,7 +3579,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3710,8 +3713,8 @@
       <c r="E7" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F7" s="73" t="s">
-        <v>123</v>
+      <c r="F7" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3728,8 +3731,8 @@
       <c r="E8" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="73" t="s">
-        <v>123</v>
+      <c r="F8" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3746,8 +3749,8 @@
       <c r="E9" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F9" s="73" t="s">
-        <v>123</v>
+      <c r="F9" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3766,7 +3769,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3945,8 +3948,8 @@
       <c r="E10" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>123</v>
+      <c r="F10" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3962,8 +3965,8 @@
       <c r="E11" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>123</v>
+      <c r="F11" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3979,8 +3982,8 @@
       <c r="E12" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>123</v>
+      <c r="F12" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3996,8 +3999,8 @@
       <c r="E13" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>123</v>
+      <c r="F13" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4013,8 +4016,8 @@
       <c r="E14" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>123</v>
+      <c r="F14" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4030,8 +4033,8 @@
       <c r="E15" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F15" s="24" t="s">
-        <v>123</v>
+      <c r="F15" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4049,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4418,7 +4421,7 @@
         <v>270</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4435,7 +4438,7 @@
         <v>270</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4452,7 +4455,7 @@
         <v>270</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4469,7 +4472,7 @@
         <v>270</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4486,7 +4489,7 @@
         <v>270</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4503,7 +4506,7 @@
         <v>270</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4520,7 +4523,7 @@
         <v>270</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4537,7 +4540,7 @@
         <v>270</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4554,7 +4557,7 @@
         <v>270</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4571,7 +4574,7 @@
         <v>270</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4588,7 +4591,7 @@
         <v>270</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4605,7 +4608,7 @@
         <v>270</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4622,7 +4625,7 @@
         <v>270</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4639,7 +4642,7 @@
         <v>270</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4656,7 +4659,7 @@
         <v>270</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4673,7 +4676,7 @@
         <v>270</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDM-6632: Reverted the excel sheet which was popping up in PR.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8C67D-A42D-774C-A18F-76AEBEF7844D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126ABC67-9A6A-D34B-A7B1-1630FC5CCD1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -904,9 +904,6 @@
   </si>
   <si>
     <t>befta.citizen.2@gmail.com</t>
-  </si>
-  <si>
-    <t>CR</t>
   </si>
 </sst>
 </file>
@@ -3357,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3476,7 +3473,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3560,7 +3557,7 @@
         <v>270</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>281</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3579,7 +3576,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3713,8 +3710,8 @@
       <c r="E7" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>281</v>
+      <c r="F7" s="73" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3731,8 +3728,8 @@
       <c r="E8" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>281</v>
+      <c r="F8" s="73" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3749,8 +3746,8 @@
       <c r="E9" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>281</v>
+      <c r="F9" s="73" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +3766,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3948,8 +3945,8 @@
       <c r="E10" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>281</v>
+      <c r="F10" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3965,8 +3962,8 @@
       <c r="E11" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>281</v>
+      <c r="F11" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3982,8 +3979,8 @@
       <c r="E12" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>281</v>
+      <c r="F12" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3999,8 +3996,8 @@
       <c r="E13" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>281</v>
+      <c r="F13" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4016,8 +4013,8 @@
       <c r="E14" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>281</v>
+      <c r="F14" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4033,8 +4030,8 @@
       <c r="E15" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>281</v>
+      <c r="F15" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4052,8 +4049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4421,7 +4418,7 @@
         <v>270</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4438,7 +4435,7 @@
         <v>270</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4455,7 +4452,7 @@
         <v>270</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4472,7 +4469,7 @@
         <v>270</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4489,7 +4486,7 @@
         <v>270</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4506,7 +4503,7 @@
         <v>270</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4523,7 +4520,7 @@
         <v>270</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4540,7 +4537,7 @@
         <v>270</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4557,7 +4554,7 @@
         <v>270</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4574,7 +4571,7 @@
         <v>270</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4591,7 +4588,7 @@
         <v>270</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4608,7 +4605,7 @@
         <v>270</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4625,7 +4622,7 @@
         <v>270</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4642,7 +4639,7 @@
         <v>270</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4659,7 +4656,7 @@
         <v>270</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,7 +4673,7 @@
         <v>270</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDM-6386: Initial checkin for the Case creation by Solicitor2.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAABC951-1B27-064C-9CA5-55532B41E542}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAF8EC5-FFC2-0949-9888-CC55363250C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3571,8 +3571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3720,7 +3720,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4638,8 +4638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6027,7 +6027,7 @@
         <v>306</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6044,7 +6044,7 @@
         <v>306</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6061,7 +6061,7 @@
         <v>306</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6078,7 +6078,7 @@
         <v>306</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6095,7 +6095,7 @@
         <v>306</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6112,7 +6112,7 @@
         <v>306</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6583,8 +6583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:F24"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-6386: Added a positive read scenario.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAF8EC5-FFC2-0949-9888-CC55363250C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8E9A1-6811-7642-8743-10227809D94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -988,6 +988,12 @@
   </si>
   <si>
     <t>befta.caseworker.2.solicitor.2@gmail.com</t>
+  </si>
+  <si>
+    <t>caseworker-befta_jurisdiction_2-solicitor_3</t>
+  </si>
+  <si>
+    <t>befta.caseworker.2.solicitor.3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1402,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1515,6 +1521,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3571,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3691,12 +3701,22 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="71"/>
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="24"/>
+      <c r="C8" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3704,6 +3724,7 @@
     <hyperlink ref="C6" r:id="rId2" xr:uid="{7AC3874F-BDAE-2D41-B77A-B32A5434DC31}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{7A87C9B7-5777-4145-9A50-F8A893972F50}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{977DB4FA-BE1F-B549-823A-29002CF2981B}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{350FA403-4E09-CF48-986D-AD9F992A88E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3717,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3828,12 +3849,27 @@
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D8" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3850,10 +3886,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E18" sqref="E16:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4135,6 +4171,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="87"/>
+      <c r="C16" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="87"/>
+      <c r="C17" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F17" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="87"/>
+      <c r="C18" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4148,10 +4238,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4623,6 +4713,162 @@
         <v>123</v>
       </c>
     </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E44" s="24"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="24"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E46" s="24"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47" s="24"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E48" s="24"/>
+    </row>
+    <row r="49" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E49" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4636,10 +4882,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4949,13 +5195,13 @@
         <v>271</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>275</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4966,13 +5212,13 @@
         <v>271</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>275</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4982,14 +5228,14 @@
       <c r="C20" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D20" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>275</v>
+      <c r="D20" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4999,14 +5245,14 @@
       <c r="C21" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D21" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>275</v>
+      <c r="D21" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5016,14 +5262,14 @@
       <c r="C22" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D22" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>275</v>
+      <c r="D22" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5034,13 +5280,13 @@
         <v>271</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>275</v>
+        <v>142</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5052,12 +5298,12 @@
         <v>271</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="F24" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="F24" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5069,10 +5315,10 @@
         <v>271</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>275</v>
+        <v>148</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>123</v>
@@ -5086,10 +5332,10 @@
         <v>271</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>275</v>
+        <v>156</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>123</v>
@@ -5102,8 +5348,8 @@
       <c r="C27" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D27" s="28" t="s">
-        <v>133</v>
+      <c r="D27" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>305</v>
@@ -5119,8 +5365,8 @@
       <c r="C28" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>135</v>
+      <c r="D28" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>305</v>
@@ -5136,8 +5382,8 @@
       <c r="C29" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>137</v>
+      <c r="D29" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>305</v>
@@ -5154,7 +5400,7 @@
         <v>271</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>305</v>
@@ -5170,8 +5416,8 @@
       <c r="C31" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D31" s="41" t="s">
-        <v>144</v>
+      <c r="D31" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>305</v>
@@ -5188,7 +5434,7 @@
         <v>271</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>305</v>
@@ -5205,7 +5451,7 @@
         <v>271</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>305</v>
@@ -5222,13 +5468,13 @@
         <v>271</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5239,13 +5485,13 @@
         <v>271</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>123</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5256,13 +5502,13 @@
         <v>271</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>123</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5273,13 +5519,13 @@
         <v>271</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>123</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5289,14 +5535,14 @@
       <c r="C38" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D38" s="24" t="s">
-        <v>235</v>
+      <c r="D38" s="41" t="s">
+        <v>282</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>123</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5307,13 +5553,13 @@
         <v>271</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>123</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5324,7 +5570,7 @@
         <v>271</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>305</v>
@@ -5341,7 +5587,7 @@
         <v>271</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>305</v>
@@ -5358,13 +5604,13 @@
         <v>271</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5372,16 +5618,16 @@
         <v>42736</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5389,16 +5635,16 @@
         <v>42736</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5406,16 +5652,16 @@
         <v>42736</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D45" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5423,16 +5669,16 @@
         <v>42736</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>305</v>
+        <v>142</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5440,16 +5686,16 @@
         <v>42736</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>305</v>
+        <v>144</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5457,13 +5703,13 @@
         <v>42736</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D48" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>305</v>
+        <v>148</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F48" s="24" t="s">
         <v>123</v>
@@ -5474,13 +5720,13 @@
         <v>42736</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D49" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>305</v>
+        <v>156</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F49" s="24" t="s">
         <v>123</v>
@@ -5493,8 +5739,8 @@
       <c r="C50" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D50" s="28" t="s">
-        <v>133</v>
+      <c r="D50" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>267</v>
@@ -5510,8 +5756,8 @@
       <c r="C51" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="28" t="s">
-        <v>135</v>
+      <c r="D51" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>267</v>
@@ -5527,8 +5773,8 @@
       <c r="C52" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D52" s="28" t="s">
-        <v>137</v>
+      <c r="D52" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>267</v>
@@ -5545,7 +5791,7 @@
         <v>272</v>
       </c>
       <c r="D53" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>267</v>
@@ -5561,8 +5807,8 @@
       <c r="C54" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D54" s="41" t="s">
-        <v>144</v>
+      <c r="D54" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>267</v>
@@ -5579,7 +5825,7 @@
         <v>272</v>
       </c>
       <c r="D55" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>267</v>
@@ -5596,7 +5842,7 @@
         <v>272</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>267</v>
@@ -5613,7 +5859,7 @@
         <v>272</v>
       </c>
       <c r="D57" s="41" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="E57" s="14" t="s">
         <v>267</v>
@@ -5630,7 +5876,7 @@
         <v>272</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>267</v>
@@ -5644,13 +5890,13 @@
         <v>42736</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D59" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F59" s="24" t="s">
         <v>123</v>
@@ -5661,13 +5907,13 @@
         <v>42736</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D60" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F60" s="24" t="s">
         <v>123</v>
@@ -5678,13 +5924,13 @@
         <v>42736</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F61" s="24" t="s">
         <v>123</v>
@@ -5695,13 +5941,13 @@
         <v>42736</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D62" s="41" t="s">
-        <v>232</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>267</v>
+        <v>142</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F62" s="24" t="s">
         <v>123</v>
@@ -5712,13 +5958,13 @@
         <v>42736</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>267</v>
+        <v>144</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F63" s="24" t="s">
         <v>123</v>
@@ -5729,13 +5975,13 @@
         <v>42736</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D64" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>267</v>
+        <v>148</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F64" s="24" t="s">
         <v>123</v>
@@ -5746,13 +5992,13 @@
         <v>42736</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D65" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>267</v>
+        <v>156</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F65" s="24" t="s">
         <v>123</v>
@@ -5765,8 +6011,8 @@
       <c r="C66" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D66" s="28" t="s">
-        <v>133</v>
+      <c r="D66" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E66" s="24" t="s">
         <v>306</v>
@@ -5782,8 +6028,8 @@
       <c r="C67" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D67" s="28" t="s">
-        <v>135</v>
+      <c r="D67" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E67" s="24" t="s">
         <v>306</v>
@@ -5799,8 +6045,8 @@
       <c r="C68" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D68" s="28" t="s">
-        <v>137</v>
+      <c r="D68" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E68" s="24" t="s">
         <v>306</v>
@@ -5817,7 +6063,7 @@
         <v>271</v>
       </c>
       <c r="D69" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E69" s="24" t="s">
         <v>306</v>
@@ -5833,8 +6079,8 @@
       <c r="C70" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D70" s="41" t="s">
-        <v>144</v>
+      <c r="D70" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E70" s="24" t="s">
         <v>306</v>
@@ -5851,7 +6097,7 @@
         <v>271</v>
       </c>
       <c r="D71" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>306</v>
@@ -5868,7 +6114,7 @@
         <v>271</v>
       </c>
       <c r="D72" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>306</v>
@@ -5885,7 +6131,7 @@
         <v>271</v>
       </c>
       <c r="D73" s="41" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>306</v>
@@ -5902,7 +6148,7 @@
         <v>271</v>
       </c>
       <c r="D74" s="41" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="E74" s="24" t="s">
         <v>306</v>
@@ -5919,7 +6165,7 @@
         <v>271</v>
       </c>
       <c r="D75" s="41" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="E75" s="24" t="s">
         <v>306</v>
@@ -5936,7 +6182,7 @@
         <v>271</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E76" s="24" t="s">
         <v>306</v>
@@ -5952,8 +6198,8 @@
       <c r="C77" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D77" s="24" t="s">
-        <v>235</v>
+      <c r="D77" s="41" t="s">
+        <v>282</v>
       </c>
       <c r="E77" s="24" t="s">
         <v>306</v>
@@ -5970,7 +6216,7 @@
         <v>271</v>
       </c>
       <c r="D78" s="41" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="E78" s="24" t="s">
         <v>306</v>
@@ -5987,7 +6233,7 @@
         <v>271</v>
       </c>
       <c r="D79" s="41" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="E79" s="24" t="s">
         <v>306</v>
@@ -6004,7 +6250,7 @@
         <v>271</v>
       </c>
       <c r="D80" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E80" s="24" t="s">
         <v>306</v>
@@ -6021,7 +6267,7 @@
         <v>271</v>
       </c>
       <c r="D81" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E81" s="24" t="s">
         <v>306</v>
@@ -6037,11 +6283,11 @@
       <c r="C82" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D82" s="41" t="s">
-        <v>280</v>
+      <c r="D82" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="E82" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F82" s="24" t="s">
         <v>123</v>
@@ -6054,11 +6300,11 @@
       <c r="C83" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D83" s="41" t="s">
-        <v>281</v>
+      <c r="D83" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F83" s="24" t="s">
         <v>123</v>
@@ -6071,11 +6317,11 @@
       <c r="C84" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D84" s="41" t="s">
-        <v>282</v>
+      <c r="D84" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="E84" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F84" s="24" t="s">
         <v>123</v>
@@ -6089,10 +6335,10 @@
         <v>271</v>
       </c>
       <c r="D85" s="41" t="s">
-        <v>283</v>
+        <v>142</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F85" s="24" t="s">
         <v>123</v>
@@ -6106,10 +6352,10 @@
         <v>271</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>284</v>
+        <v>144</v>
       </c>
       <c r="E86" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F86" s="24" t="s">
         <v>123</v>
@@ -6123,10 +6369,10 @@
         <v>271</v>
       </c>
       <c r="D87" s="41" t="s">
-        <v>244</v>
+        <v>148</v>
       </c>
       <c r="E87" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F87" s="24" t="s">
         <v>123</v>
@@ -6140,12 +6386,300 @@
         <v>271</v>
       </c>
       <c r="D88" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E88" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D89" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D90" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D92" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D94" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D95" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E95" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F95" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D96" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F96" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D97" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F97" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F98" s="24" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D99" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F99" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D100" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F100" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D101" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F101" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D102" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F102" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D103" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F103" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="E88" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="F88" s="24" t="s">
+      <c r="E104" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F104" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -6162,7 +6696,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -6416,6 +6950,66 @@
         <v>306</v>
       </c>
       <c r="G12" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="80" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RDM-7087: Definition file for BEFTA Jurisdiction2 Document ACL.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAABC951-1B27-064C-9CA5-55532B41E542}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8E9A1-6811-7642-8743-10227809D94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -988,6 +988,12 @@
   </si>
   <si>
     <t>befta.caseworker.2.solicitor.2@gmail.com</t>
+  </si>
+  <si>
+    <t>caseworker-befta_jurisdiction_2-solicitor_3</t>
+  </si>
+  <si>
+    <t>befta.caseworker.2.solicitor.3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1402,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1515,6 +1521,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3572,7 +3582,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3691,12 +3701,22 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="71"/>
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="24"/>
+      <c r="C8" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3704,6 +3724,7 @@
     <hyperlink ref="C6" r:id="rId2" xr:uid="{7AC3874F-BDAE-2D41-B77A-B32A5434DC31}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{7A87C9B7-5777-4145-9A50-F8A893972F50}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{977DB4FA-BE1F-B549-823A-29002CF2981B}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{350FA403-4E09-CF48-986D-AD9F992A88E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3717,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3828,12 +3849,27 @@
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D8" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3850,10 +3886,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E18" sqref="E16:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4135,6 +4171,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="87"/>
+      <c r="C16" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="87"/>
+      <c r="C17" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F17" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="87"/>
+      <c r="C18" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4148,10 +4238,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4623,6 +4713,162 @@
         <v>123</v>
       </c>
     </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E44" s="24"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="24"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E46" s="24"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47" s="24"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E48" s="24"/>
+    </row>
+    <row r="49" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E49" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4636,10 +4882,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4949,13 +5195,13 @@
         <v>271</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>275</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4966,13 +5212,13 @@
         <v>271</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>275</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4982,14 +5228,14 @@
       <c r="C20" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D20" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>275</v>
+      <c r="D20" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4999,14 +5245,14 @@
       <c r="C21" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D21" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>275</v>
+      <c r="D21" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5016,14 +5262,14 @@
       <c r="C22" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D22" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>275</v>
+      <c r="D22" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5034,13 +5280,13 @@
         <v>271</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>275</v>
+        <v>142</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5052,12 +5298,12 @@
         <v>271</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="F24" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="F24" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5069,10 +5315,10 @@
         <v>271</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>275</v>
+        <v>148</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>123</v>
@@ -5086,10 +5332,10 @@
         <v>271</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>275</v>
+        <v>156</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>123</v>
@@ -5102,8 +5348,8 @@
       <c r="C27" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D27" s="28" t="s">
-        <v>133</v>
+      <c r="D27" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>305</v>
@@ -5119,8 +5365,8 @@
       <c r="C28" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>135</v>
+      <c r="D28" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>305</v>
@@ -5136,8 +5382,8 @@
       <c r="C29" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>137</v>
+      <c r="D29" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>305</v>
@@ -5154,7 +5400,7 @@
         <v>271</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>305</v>
@@ -5170,8 +5416,8 @@
       <c r="C31" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D31" s="41" t="s">
-        <v>144</v>
+      <c r="D31" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>305</v>
@@ -5188,7 +5434,7 @@
         <v>271</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>305</v>
@@ -5205,7 +5451,7 @@
         <v>271</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>305</v>
@@ -5222,13 +5468,13 @@
         <v>271</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5239,13 +5485,13 @@
         <v>271</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>123</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5256,13 +5502,13 @@
         <v>271</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>123</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5273,13 +5519,13 @@
         <v>271</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>123</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5289,14 +5535,14 @@
       <c r="C38" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D38" s="24" t="s">
-        <v>235</v>
+      <c r="D38" s="41" t="s">
+        <v>282</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>123</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5307,13 +5553,13 @@
         <v>271</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>123</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5324,7 +5570,7 @@
         <v>271</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>305</v>
@@ -5341,7 +5587,7 @@
         <v>271</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>305</v>
@@ -5358,13 +5604,13 @@
         <v>271</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>305</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5372,16 +5618,16 @@
         <v>42736</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5389,16 +5635,16 @@
         <v>42736</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5406,16 +5652,16 @@
         <v>42736</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D45" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>305</v>
+        <v>272</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5423,16 +5669,16 @@
         <v>42736</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>305</v>
+        <v>142</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5440,16 +5686,16 @@
         <v>42736</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>305</v>
+        <v>144</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5457,13 +5703,13 @@
         <v>42736</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D48" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>305</v>
+        <v>148</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F48" s="24" t="s">
         <v>123</v>
@@ -5474,13 +5720,13 @@
         <v>42736</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D49" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>305</v>
+        <v>156</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="F49" s="24" t="s">
         <v>123</v>
@@ -5493,8 +5739,8 @@
       <c r="C50" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D50" s="28" t="s">
-        <v>133</v>
+      <c r="D50" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>267</v>
@@ -5510,8 +5756,8 @@
       <c r="C51" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="28" t="s">
-        <v>135</v>
+      <c r="D51" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>267</v>
@@ -5527,8 +5773,8 @@
       <c r="C52" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D52" s="28" t="s">
-        <v>137</v>
+      <c r="D52" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>267</v>
@@ -5545,7 +5791,7 @@
         <v>272</v>
       </c>
       <c r="D53" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>267</v>
@@ -5561,8 +5807,8 @@
       <c r="C54" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D54" s="41" t="s">
-        <v>144</v>
+      <c r="D54" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>267</v>
@@ -5579,7 +5825,7 @@
         <v>272</v>
       </c>
       <c r="D55" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>267</v>
@@ -5596,7 +5842,7 @@
         <v>272</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>267</v>
@@ -5613,7 +5859,7 @@
         <v>272</v>
       </c>
       <c r="D57" s="41" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="E57" s="14" t="s">
         <v>267</v>
@@ -5630,7 +5876,7 @@
         <v>272</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>267</v>
@@ -5644,13 +5890,13 @@
         <v>42736</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D59" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F59" s="24" t="s">
         <v>123</v>
@@ -5661,13 +5907,13 @@
         <v>42736</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D60" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F60" s="24" t="s">
         <v>123</v>
@@ -5678,13 +5924,13 @@
         <v>42736</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F61" s="24" t="s">
         <v>123</v>
@@ -5695,13 +5941,13 @@
         <v>42736</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D62" s="41" t="s">
-        <v>232</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>267</v>
+        <v>142</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F62" s="24" t="s">
         <v>123</v>
@@ -5712,13 +5958,13 @@
         <v>42736</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>267</v>
+        <v>144</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F63" s="24" t="s">
         <v>123</v>
@@ -5729,13 +5975,13 @@
         <v>42736</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D64" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>267</v>
+        <v>148</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F64" s="24" t="s">
         <v>123</v>
@@ -5746,13 +5992,13 @@
         <v>42736</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D65" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>267</v>
+        <v>156</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>306</v>
       </c>
       <c r="F65" s="24" t="s">
         <v>123</v>
@@ -5765,8 +6011,8 @@
       <c r="C66" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D66" s="28" t="s">
-        <v>133</v>
+      <c r="D66" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="E66" s="24" t="s">
         <v>306</v>
@@ -5782,8 +6028,8 @@
       <c r="C67" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D67" s="28" t="s">
-        <v>135</v>
+      <c r="D67" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="E67" s="24" t="s">
         <v>306</v>
@@ -5799,8 +6045,8 @@
       <c r="C68" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D68" s="28" t="s">
-        <v>137</v>
+      <c r="D68" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="E68" s="24" t="s">
         <v>306</v>
@@ -5817,7 +6063,7 @@
         <v>271</v>
       </c>
       <c r="D69" s="41" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E69" s="24" t="s">
         <v>306</v>
@@ -5833,8 +6079,8 @@
       <c r="C70" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D70" s="41" t="s">
-        <v>144</v>
+      <c r="D70" s="24" t="s">
+        <v>235</v>
       </c>
       <c r="E70" s="24" t="s">
         <v>306</v>
@@ -5851,7 +6097,7 @@
         <v>271</v>
       </c>
       <c r="D71" s="41" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>306</v>
@@ -5868,7 +6114,7 @@
         <v>271</v>
       </c>
       <c r="D72" s="41" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E72" s="24" t="s">
         <v>306</v>
@@ -5885,7 +6131,7 @@
         <v>271</v>
       </c>
       <c r="D73" s="41" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>306</v>
@@ -5902,7 +6148,7 @@
         <v>271</v>
       </c>
       <c r="D74" s="41" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="E74" s="24" t="s">
         <v>306</v>
@@ -5919,7 +6165,7 @@
         <v>271</v>
       </c>
       <c r="D75" s="41" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="E75" s="24" t="s">
         <v>306</v>
@@ -5936,7 +6182,7 @@
         <v>271</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E76" s="24" t="s">
         <v>306</v>
@@ -5952,8 +6198,8 @@
       <c r="C77" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D77" s="24" t="s">
-        <v>235</v>
+      <c r="D77" s="41" t="s">
+        <v>282</v>
       </c>
       <c r="E77" s="24" t="s">
         <v>306</v>
@@ -5970,7 +6216,7 @@
         <v>271</v>
       </c>
       <c r="D78" s="41" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="E78" s="24" t="s">
         <v>306</v>
@@ -5987,7 +6233,7 @@
         <v>271</v>
       </c>
       <c r="D79" s="41" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="E79" s="24" t="s">
         <v>306</v>
@@ -6004,7 +6250,7 @@
         <v>271</v>
       </c>
       <c r="D80" s="41" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="E80" s="24" t="s">
         <v>306</v>
@@ -6021,13 +6267,13 @@
         <v>271</v>
       </c>
       <c r="D81" s="41" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E81" s="24" t="s">
         <v>306</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6037,14 +6283,14 @@
       <c r="C82" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D82" s="41" t="s">
-        <v>280</v>
+      <c r="D82" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="E82" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>297</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6054,14 +6300,14 @@
       <c r="C83" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D83" s="41" t="s">
-        <v>281</v>
+      <c r="D83" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>295</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6071,14 +6317,14 @@
       <c r="C84" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D84" s="41" t="s">
-        <v>282</v>
+      <c r="D84" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="E84" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>294</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6089,13 +6335,13 @@
         <v>271</v>
       </c>
       <c r="D85" s="41" t="s">
-        <v>283</v>
+        <v>142</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6106,13 +6352,13 @@
         <v>271</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>284</v>
+        <v>144</v>
       </c>
       <c r="E86" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6123,10 +6369,10 @@
         <v>271</v>
       </c>
       <c r="D87" s="41" t="s">
-        <v>244</v>
+        <v>148</v>
       </c>
       <c r="E87" s="24" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F87" s="24" t="s">
         <v>123</v>
@@ -6140,12 +6386,300 @@
         <v>271</v>
       </c>
       <c r="D88" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E88" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D89" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D90" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D92" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D94" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D95" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E95" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F95" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D96" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F96" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D97" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F97" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F98" s="24" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D99" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F99" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D100" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F100" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D101" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F101" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D102" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F102" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D103" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F103" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="E88" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="F88" s="24" t="s">
+      <c r="E104" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="F104" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -6162,7 +6696,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -6416,6 +6950,66 @@
         <v>306</v>
       </c>
       <c r="G12" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="80" t="s">
         <v>123</v>
       </c>
     </row>
@@ -6583,8 +7177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:F24"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-7068:  Dummy update in the excel file
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/566377/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8E9A1-6811-7642-8743-10227809D94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381204F-69C8-F84A-8A84-71C495A7F25D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3581,7 +3581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -4240,7 +4240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -4884,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5882,7 +5882,7 @@
         <v>267</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>123</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
AM-439: S-578 data files.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8E9A1-6811-7642-8743-10227809D94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D881EAD-CAA8-9048-AE5E-C017AAEB6A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1860,7 +1860,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1956,7 +1956,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2413,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="C19:H25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3581,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3738,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3873,6 +3873,21 @@
         <v>123</v>
       </c>
     </row>
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3886,10 +3901,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E16:E18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4225,6 +4240,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="19" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="52"/>
+      <c r="C19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4240,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4821,23 +4890,107 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E39" s="24"/>
+    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E40" s="24"/>
@@ -4882,10 +5035,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6680,6 +6833,404 @@
         <v>309</v>
       </c>
       <c r="F104" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D105" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D106" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F106" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D107" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D108" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F108" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D109" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D110" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F110" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D111" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F111" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D112" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F112" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F113" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D114" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D115" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F115" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D116" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F116" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D117" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F117" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D119" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E119" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F119" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D120" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F120" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D121" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E121" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D122" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F122" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D123" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E123" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F123" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D124" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F124" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D125" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F125" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D126" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F126" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D127" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F127" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -7023,7 +7574,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8461,7 +9012,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8705,7 +9256,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8997,7 +9548,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9205,7 +9756,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C9"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9810,8 +10361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E25"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13667,7 +14218,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-7071: Updated S-578: Added new scenario and data files.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/566377/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381204F-69C8-F84A-8A84-71C495A7F25D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDF7373-EF25-C34A-9E3B-CE9B000FACFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="19420" windowHeight="16480" tabRatio="823" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2414,7 +2414,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="C19:H25"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3582,7 +3582,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3738,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3873,6 +3873,21 @@
         <v>123</v>
       </c>
     </row>
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3886,10 +3901,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E16:E18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4225,6 +4240,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="19" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="52"/>
+      <c r="C19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4240,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4821,23 +4890,107 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E39" s="24"/>
+    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E40" s="24"/>
@@ -4882,10 +5035,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6680,6 +6833,397 @@
         <v>309</v>
       </c>
       <c r="F104" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D105" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D106" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F106" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D107" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D108" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F108" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D109" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D110" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F110" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D111" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F111" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D112" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F112" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F113" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D114" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D115" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F115" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D116" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F116" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D117" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F117" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D119" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E119" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F119" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D120" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F120" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D121" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E121" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D122" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F122" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D123" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E123" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F123" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D124" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F124" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D125" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F125" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D126" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F126" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D127" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F127" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -6698,8 +7242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7177,8 +7721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:G24"/>
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8705,7 +9249,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9205,7 +9749,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C9"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9810,8 +10354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E25"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13666,8 +14210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-6386: Fixed the code.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8E9A1-6811-7642-8743-10227809D94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,9 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseField!$A$1:$F$111</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3581,8 +3584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3738,10 +3741,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3864,12 +3867,27 @@
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>267</v>
       </c>
       <c r="E8" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3886,10 +3904,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E16:E18"/>
+      <selection activeCell="A19" sqref="A19:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4225,6 +4243,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="87"/>
+      <c r="C19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="87"/>
+      <c r="C20" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="87"/>
+      <c r="C21" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4240,8 +4312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4822,22 +4894,112 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E34" s="24"/>
+      <c r="A34" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E35" s="24"/>
+      <c r="A35" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E36" s="24"/>
+      <c r="A36" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E37" s="24"/>
+      <c r="A37" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E38" s="24"/>
+      <c r="A38" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E39" s="24"/>
+      <c r="A39" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E40" s="24"/>
@@ -4882,10 +5044,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F104"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119:D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4912,7 +5075,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -4928,7 +5091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" s="32" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>8</v>
       </c>
@@ -5613,7 +5776,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="71">
         <v>42736</v>
       </c>
@@ -5630,7 +5793,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="71">
         <v>42736</v>
       </c>
@@ -5647,7 +5810,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="71">
         <v>42736</v>
       </c>
@@ -5664,7 +5827,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="71">
         <v>42736</v>
       </c>
@@ -5681,7 +5844,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="71">
         <v>42736</v>
       </c>
@@ -5698,7 +5861,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="71">
         <v>42736</v>
       </c>
@@ -5715,7 +5878,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="71">
         <v>42736</v>
       </c>
@@ -5732,7 +5895,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="71">
         <v>42736</v>
       </c>
@@ -5749,7 +5912,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="71">
         <v>42736</v>
       </c>
@@ -5766,7 +5929,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="71">
         <v>42736</v>
       </c>
@@ -5783,7 +5946,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="71">
         <v>42736</v>
       </c>
@@ -5800,7 +5963,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="71">
         <v>42736</v>
       </c>
@@ -5817,7 +5980,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="71">
         <v>42736</v>
       </c>
@@ -5834,7 +5997,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="71">
         <v>42736</v>
       </c>
@@ -5851,7 +6014,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="71">
         <v>42736</v>
       </c>
@@ -5868,7 +6031,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="71">
         <v>42736</v>
       </c>
@@ -6683,7 +6846,428 @@
         <v>123</v>
       </c>
     </row>
+    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F106" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D107" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D108" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F108" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D109" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D110" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F110" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D111" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F111" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D112" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F112" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D113" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F113" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B114" s="14"/>
+      <c r="C114" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D114" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D115" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F115" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B116" s="14"/>
+      <c r="C116" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D116" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F116" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D117" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F117" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B118" s="14"/>
+      <c r="C118" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D119" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E119" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F119" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D120" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F120" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B121" s="14"/>
+      <c r="C121" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D121" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E121" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B122" s="14"/>
+      <c r="C122" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D122" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F122" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B123" s="14"/>
+      <c r="C123" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D123" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="E123" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F123" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D124" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F124" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B125" s="14"/>
+      <c r="C125" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D125" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F125" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B126" s="14"/>
+      <c r="C126" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D126" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F126" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D127" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F127" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F111" xr:uid="{562AAE8F-3145-EE4D-AFA6-9179B8265258}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="BEFTA_CASETYPE_2_1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -6696,10 +7280,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7012,6 +7596,27 @@
       <c r="G15" s="80" t="s">
         <v>123</v>
       </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="71"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="71"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="71"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7177,8 +7782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:G24"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-7071: Updated data files as per review comments.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDBC91C-643A-E344-B7BD-49E84E823333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D7BAD3-BD1A-D046-8B2D-9A23395AD638}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5037,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6851,7 +6851,7 @@
         <v>267</v>
       </c>
       <c r="F105" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6887,7 +6887,7 @@
         <v>267</v>
       </c>
       <c r="F107" s="24" t="s">
-        <v>123</v>
+        <v>294</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6923,7 +6923,7 @@
         <v>267</v>
       </c>
       <c r="F109" s="24" t="s">
-        <v>123</v>
+        <v>297</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6941,7 +6941,7 @@
         <v>267</v>
       </c>
       <c r="F110" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6959,7 +6959,7 @@
         <v>267</v>
       </c>
       <c r="F111" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
RDM-7072: Submit event creation for citizen document
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B35D2ED-2BE0-F64E-8701-516DA9A2AB20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5047,8 +5047,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119:F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7113,7 +7113,7 @@
         <v>267</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7131,7 +7131,7 @@
         <v>267</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7149,7 +7149,7 @@
         <v>267</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7185,7 +7185,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7203,7 +7203,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7221,7 +7221,7 @@
         <v>267</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7282,7 +7282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-7071: Added new scenario and data files.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B71DE8-E636-1640-8018-5733A0B89AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12900" yWindow="-21320" windowWidth="28800" windowHeight="16480" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5047,8 +5047,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7113,7 +7113,7 @@
         <v>267</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7131,7 +7131,7 @@
         <v>267</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7149,7 +7149,7 @@
         <v>267</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7185,7 +7185,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7203,7 +7203,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7221,7 +7221,7 @@
         <v>267</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7282,7 +7282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-7222: Updated the common citizen case creation files.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B71DE8-E636-1640-8018-5733A0B89AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12900" yWindow="-21320" windowWidth="28800" windowHeight="16480" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5047,8 +5047,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7113,7 +7113,7 @@
         <v>267</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7131,7 +7131,7 @@
         <v>267</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7149,7 +7149,7 @@
         <v>267</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7185,7 +7185,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7203,7 +7203,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7221,7 +7221,7 @@
         <v>267</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7282,7 +7282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-7072-Submit-event-creation-as-Citizen - Updated excel file with right permissions for citizen
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26AACA2-0136-034D-B20E-1BCD5F8E6D7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5047,8 +5047,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119:F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7113,7 +7113,7 @@
         <v>267</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>123</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7131,7 +7131,7 @@
         <v>267</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7149,7 +7149,7 @@
         <v>267</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7185,7 +7185,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7203,7 +7203,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7221,7 +7221,7 @@
         <v>267</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7282,7 +7282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>